<commit_message>
added code toadd status adn accuracy
</commit_message>
<xml_diff>
--- a/LOGS/a5f6da06-f864-4636-80e8-db4a1edb1e66/main_page_service_output/notes_transformed_standard_cropped_df.xlsx
+++ b/LOGS/a5f6da06-f864-4636-80e8-db4a1edb1e66/main_page_service_output/notes_transformed_standard_cropped_df.xlsx
@@ -44,19 +44,19 @@
     <t>10 Inventories Provision for inventory obsolescence</t>
   </si>
   <si>
-    <t xml:space="preserve">10 Inventories </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Trade payables</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Amounts payable to controlling entity (Refer Note 19)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Other creditors and accruals</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <t>10 Inventories nan</t>
+  </si>
+  <si>
+    <t>None Trade payables</t>
+  </si>
+  <si>
+    <t>None Amounts payable to controlling entity (Refer Note 19)</t>
+  </si>
+  <si>
+    <t>None Other creditors and accruals</t>
+  </si>
+  <si>
+    <t>None nan</t>
   </si>
   <si>
     <t>Trade and other payables</t>
@@ -95,22 +95,22 @@
     <t>Current Liability for annual leave and other current employee benefits</t>
   </si>
   <si>
-    <t xml:space="preserve">Current </t>
+    <t>Current nan</t>
   </si>
   <si>
     <t>Non-current Liability for long-service leave</t>
   </si>
   <si>
-    <t xml:space="preserve">Non-current </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> at 1 January</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> at31 December</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> at 31 December</t>
+    <t>Non-current nan</t>
+  </si>
+  <si>
+    <t>None at 1 January</t>
+  </si>
+  <si>
+    <t>None at31 December</t>
+  </si>
+  <si>
+    <t>None at 31 December</t>
   </si>
   <si>
     <t>A class ordinary shares Shares</t>
@@ -119,19 +119,19 @@
     <t>Aclass ordinary shares $'000</t>
   </si>
   <si>
-    <t xml:space="preserve"> On issue at 1 January</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> On issue at 31 December</t>
+    <t>None On issue at 1 January</t>
+  </si>
+  <si>
+    <t>None On issue at 31 December</t>
   </si>
   <si>
     <t>Total $'000</t>
   </si>
   <si>
-    <t xml:space="preserve"> Cents per share (fully franked)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Total dollar amount</t>
+    <t>None Cents per share (fully franked)</t>
+  </si>
+  <si>
+    <t>None Total dollar amount</t>
   </si>
   <si>
     <t>$</t>

</xml_diff>